<commit_message>
Added: Ejecutador.bat Update: Automatizacion -> Se agrego nueva funcion para usar whats template
</commit_message>
<xml_diff>
--- a/Read/Datos.xlsx
+++ b/Read/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mate9\OneDrive - talent.com\Proyectos Node\Automatizacion Rudy\Read\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8710D831-D258-449C-8F29-D1E5CD4B9891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88006A9A-155A-4594-959D-F38E4176E2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Macro Plantilla" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="169">
   <si>
     <t>Telefono</t>
   </si>
@@ -38,9 +39,6 @@
   </si>
   <si>
     <t>Esto es un mensaje de prueba #2</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>Template What</t>
@@ -592,27 +590,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -623,19 +601,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF98D8C9-2873-47BF-9747-DB53C60653E9}" name="Table1" displayName="Table1" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:C1048576" xr:uid="{CF98D8C9-2873-47BF-9747-DB53C60653E9}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{84C62015-93B2-436B-86EB-078E2438A1AB}" name="Telefono" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{3F656B3D-F214-48ED-9D14-525362E25770}" name="Template What" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6DEB1A64-718F-4928-A737-FBEEE24991F2}" name="Mensaje" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{D55A8A89-FDF2-473E-8E6B-D766ACDF1284}" name="Column2" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -930,7 +895,7 @@
         <v>18015749359</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -941,7 +906,7 @@
         <v>13185737090</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -952,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -963,7 +928,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -974,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>3</v>
@@ -985,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>4</v>
@@ -996,17 +961,95 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1014,7 +1057,7 @@
           <x14:formula1>
             <xm:f>'Macro Plantilla'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8</xm:sqref>
+          <xm:sqref>B2:B35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1037,822 +1080,822 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>